<commit_message>
first draft of extraction complete
</commit_message>
<xml_diff>
--- a/extraction.xlsx
+++ b/extraction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/covid-litsearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123089CD-6D94-684B-BC59-EFBDBDADB045}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64774CA2-4376-6C4B-A07A-57FDA02E5975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{9E52B812-410C-D44B-8095-C72A873F12D0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="133">
   <si>
     <t>Author</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Ackland</t>
   </si>
   <si>
-    <t>"UK" in abstract</t>
-  </si>
-  <si>
     <t>Arxiv</t>
   </si>
   <si>
@@ -291,6 +288,150 @@
   </si>
   <si>
     <t>No, except for ratio between critical care and total cases</t>
+  </si>
+  <si>
+    <t>A lot of input data on contacts, population and age distribution, school holidays, etc, but only roughly fit to deaths. (To read appendix for more detail).</t>
+  </si>
+  <si>
+    <t>350000 (170000-480000) deaths to December 2021 if unmitigated (not accounting for additional fatality due to exceeded hospital capacity). Under intensive intervention for 12 weeks, 120000 (27000-260000 deaths).</t>
+  </si>
+  <si>
+    <t>23 million (13-30 million) cases to December 2021 if unmitigated. 11 millio cases (1.9-20 million) under intensive intervention for 12 weeks.</t>
+  </si>
+  <si>
+    <t>Up to December 2021</t>
+  </si>
+  <si>
+    <t>Peak ICU beds reported, will check in appendix for more detail</t>
+  </si>
+  <si>
+    <t>Published 2 June 2020 but data seem to be based on end of March.</t>
+  </si>
+  <si>
+    <t>Stochastic age structured transmission model also geographic structure. Accounts for transmission between different age groups based on UK social mixing patterns. Uncertainty with 200 runs for each scenario, random values of R0 and seeding chosen. Looks like a good model done by experienced people, but I need to read appendix in detail.</t>
+  </si>
+  <si>
+    <t>Published 12 May 2020</t>
+  </si>
+  <si>
+    <t>School closures, physical distancing, shielding older people, self-isolation, and combination of all four, compared to baseline. Also look at timing of implementing interventions. Also simulated lockdown as imposed from 16 March (assuming 12 weeks). DOES NOT ACCOUNT FOR MEASURES ANNOUNCED 23 MARCH.</t>
+  </si>
+  <si>
+    <t>Yes - but maybe for baseline only.</t>
+  </si>
+  <si>
+    <t>Excess mortality calculation compared for mitigation vs full suppression. Risk calculator online. Based on linked health records calculate all cause mortality at 1 year for a variety of risk factors, and then calculate excess deaths over 1 year under different scenarios. The model of baseline mortality seems more robust than the estimate of Covid-related deaths.</t>
+  </si>
+  <si>
+    <t>Data from England extrapolated to UK</t>
+  </si>
+  <si>
+    <t>Data on prevalence of risk factors and fatality rate over 1 year for each from clinical data, then calculate risk ratio for deaths from covid (present a range of RR), and apply this to a % of people assumed to be infected.</t>
+  </si>
+  <si>
+    <t>Assume certain % of people eventually infected under a variety of scenarios: 0.001% for full suppression scenario, 1% for partial suppression, 10% for mitigation, 80% for do nothing</t>
+  </si>
+  <si>
+    <t>To January 2021 I think (1 year)</t>
+  </si>
+  <si>
+    <t>Only present excess deaths, ranging from 58,798  to 587,982 under do nothing scenario, to 1-7 excess deaths under full suppression. Partial suppression 735-7350, Mitigation 7350-73498.</t>
+  </si>
+  <si>
+    <t>Yes, could use to crosscheck excess deaths according to % of population eventually infected</t>
+  </si>
+  <si>
+    <t>Published 15 June 2020</t>
+  </si>
+  <si>
+    <t>Use for % of population at high risk with underlying conditions (though Banarjee also presents this more specifically for UK)</t>
+  </si>
+  <si>
+    <t>Global mapping of conditions considered important comorbidities for covid</t>
+  </si>
+  <si>
+    <t>Worldometer data</t>
+  </si>
+  <si>
+    <t>UK and others</t>
+  </si>
+  <si>
+    <t>Data up to 24 April 2020</t>
+  </si>
+  <si>
+    <t>Fit ARIMA model to data o cases, deaths, and recoveries. Project over 60 days forward (to 7 July). High uncertainty in projections and no mechanistic assumptions of how it will change over time.</t>
+  </si>
+  <si>
+    <t>medRxiv and preprint on PubMed because NIH funded</t>
+  </si>
+  <si>
+    <t>Fit SIR model to infection and death in 9 countries, identify parameters that are similar and different between the countries. Very simple model used for more of a modelling exercise than for prediction.</t>
+  </si>
+  <si>
+    <t>UK and other European countries</t>
+  </si>
+  <si>
+    <t>Ferguson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theoretical interventions as done before any interventions implemented. Assume all policies in place for 3-5 months. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">individual based model originally developed for flu which includes contact tracing data. </t>
+  </si>
+  <si>
+    <t>Assumptions about incubation, infectiousness, R0 based on Wuhan. Fit to data on cumulative number of deaths by 14 March.</t>
+  </si>
+  <si>
+    <t>Up to October 2020</t>
+  </si>
+  <si>
+    <t>Baseline 510,000. Many alternative mitigation strategies presented, so need to decide which to pull out.</t>
+  </si>
+  <si>
+    <t>Yes but maybe more recent ones better</t>
+  </si>
+  <si>
+    <t>Excess deaths calculated compared to expected deaths based on statistical model for deaths 2010-2020. Calculated up to 5 June 2020.</t>
+  </si>
+  <si>
+    <t>Another calculation of excess deaths, broken down by age groups</t>
+  </si>
+  <si>
+    <t>"UK" in abstract (on medRxiv)</t>
+  </si>
+  <si>
+    <t>Take Imperial model and reparameterize to additional time. Present 10 stochastic simulations for each scenario.Useful for narrowing down which presented results from Report 9 to use.</t>
+  </si>
+  <si>
+    <t>Alongside Report 9 to narrow down useful scenarios/parameter values.</t>
+  </si>
+  <si>
+    <t>Last update 29 June (updated frequently)</t>
+  </si>
+  <si>
+    <t>UK (and others)</t>
+  </si>
+  <si>
+    <t>Projected forward from today  using observed deaths, daily infections and testing until 1 October 2020.</t>
+  </si>
+  <si>
+    <t>Current projection, mandates easing, masks required.</t>
+  </si>
+  <si>
+    <t>Current: 47,924 (46,131-50,319); Easing 47,962 (46,131 - 50,319); Masks 45,395 (44,790-46,113)</t>
+  </si>
+  <si>
+    <t>To 1 October 2020</t>
+  </si>
+  <si>
+    <t>Only show daily, not cumulative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I haven't found any details on this yet. </t>
+  </si>
+  <si>
+    <t>Maybe. Scenarios presented are very up to date and there is uncertainty in projections. But unsure of methods.</t>
   </si>
 </sst>
 </file>
@@ -650,10 +791,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31061C2-8AFA-1A45-84DA-162895B78F7C}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="186" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="186" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,12 +802,14 @@
     <col min="1" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="31.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="27.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="21.1640625" style="1" customWidth="1"/>
-    <col min="10" max="12" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="21" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="1"/>
     <col min="13" max="13" width="17.6640625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -676,7 +819,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -685,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -720,10 +863,10 @@
     </row>
     <row r="2" spans="1:15" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -732,39 +875,39 @@
         <v>43999</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="2">
         <v>44074</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
@@ -773,27 +916,27 @@
         <v>43991</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
@@ -802,27 +945,27 @@
         <v>44000</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="136" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -831,16 +974,16 @@
         <v>43963</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I5" s="1">
         <v>39000</v>
@@ -849,15 +992,15 @@
         <v>252000</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="221" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -866,30 +1009,30 @@
         <v>43959</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -898,21 +1041,21 @@
         <v>43916</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="153" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -921,36 +1064,36 @@
         <v>43988</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
@@ -959,30 +1102,30 @@
         <v>43961</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="O9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="204" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -991,24 +1134,24 @@
         <v>43978</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
@@ -1017,67 +1160,250 @@
         <v>43936</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" ht="145" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="D12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="204" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="D15" s="2">
+        <v>43979</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="153" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="C16" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="136" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="D17" s="2">
         <v>43906</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E17" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="D18" s="2">
         <v>44000</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E18" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>121</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="D20" s="2">
+        <v>44004</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some kind of update to extraction
</commit_message>
<xml_diff>
--- a/extraction.xlsx
+++ b/extraction.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/covid-litsearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199A6243-CE1B-9441-B24C-3E353C1F1694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A30655-61D2-F942-862F-840743CE58C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="1" xr2:uid="{73474356-85FC-2C44-83A7-B203B79C5057}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{73474356-85FC-2C44-83A7-B203B79C5057}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="197">
   <si>
     <t>Author</t>
   </si>
@@ -621,10 +621,10 @@
     <t>CI_HQ_SD</t>
   </si>
   <si>
+    <t>PC_CI_SD</t>
+  </si>
+  <si>
     <t>PC_CI_HQ_SD [all 4 interventions, case isolation, home quarantine, social distancing, school closure, these have all been used]</t>
-  </si>
-  <si>
-    <t>PC_CI_SD [this seems most similar in outcome to Banarjee's mitigation strategy]</t>
   </si>
 </sst>
 </file>
@@ -1684,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70F69A0-FAED-784F-B2D4-C2A53A6FD9D8}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2222,19 +2222,25 @@
       <c r="E26">
         <v>120000</v>
       </c>
+      <c r="J26" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>111</v>
       </c>
       <c r="B27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D27">
         <v>6400</v>
       </c>
       <c r="E27">
         <v>71000</v>
+      </c>
+      <c r="J27" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -2242,13 +2248,16 @@
         <v>111</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D28">
         <v>5600</v>
       </c>
       <c r="E28">
         <v>48000</v>
+      </c>
+      <c r="J28" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did some more full text screening
</commit_message>
<xml_diff>
--- a/extraction.xlsx
+++ b/extraction.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/covid-litsearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A30655-61D2-F942-862F-840743CE58C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0024107-121B-C241-9BD4-59026F07E0B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{73474356-85FC-2C44-83A7-B203B79C5057}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Other countries" sheetId="3" r:id="rId2"/>
+    <sheet name="UK" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="366">
   <si>
     <t>Author</t>
   </si>
@@ -625,6 +626,658 @@
   </si>
   <si>
     <t>PC_CI_HQ_SD [all 4 interventions, case isolation, home quarantine, social distancing, school closure, these have all been used]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Sensitivity analysis of the effects of non-pharmaceutical interventions on COVID-19 in Europe 
+</t>
+  </si>
+  <si>
+    <t>Soltesz, K.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.06.15.20131953v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Modelling of the second (and subsequent) waves of the coronavirus epidemic. Spain and Germany as case studies 
+</t>
+  </si>
+  <si>
+    <t>de Castro, F.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.06.12.20129429v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+How did governmental interventions affect the spread of COVID-19 in European countries? 
+</t>
+  </si>
+  <si>
+    <t>Post, R. A. J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.27.20114272v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Predictions for Europe for the Covid-19 pandemic from a SIR model 
+</t>
+  </si>
+  <si>
+    <t>Bhanot, G.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.26.20114058v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Six Scenarios for non-medical interventions in the SARS-CoV-2 epidemic 
+</t>
+  </si>
+  <si>
+    <t>Kempf, P.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.25.20112532v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The effect of multiple interventions to balance healthcare demand for controlling COVID-19 outbreaks: a modelling study 
+</t>
+  </si>
+  <si>
+    <t>Yang, P.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.19.20107326v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+European lockdowns and the consequences of relaxation during the COVID-19 pandemic 
+</t>
+  </si>
+  <si>
+    <t>Glass, D. H.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.19.20106542v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Hasty Reduction of COVID-19 Lockdown Measures Leads to the Second Wave of Infection 
+</t>
+  </si>
+  <si>
+    <t>Hazem, Y.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.23.20111526v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Data-driven analysis on the simulations of the spread of COVID-19 under different interventions of China 
+</t>
+  </si>
+  <si>
+    <t>Tian, T.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.15.20103051v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+An integrated deterministic-stochastic approach for predicting the long-term trajectories of COVID-19 
+</t>
+  </si>
+  <si>
+    <t>Chakraborty, T.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.13.20101303v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The Clinical and Economic Value of a Successful Shutdown During the SARS-CoV-2 Pandemic in Germany 
+</t>
+  </si>
+  <si>
+    <t>Gandjour, A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.12.20098996v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Relaxing lockdown measures in epidemic outbreaks using selective socio-economic containment with uncertainty 
+</t>
+  </si>
+  <si>
+    <t>Albi, G.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.12.20099721v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+COVID-19: Predictive Mathematical Models for the Number of Deaths in South Korea, Italy, Spain, France, UK, Germany, and USA 
+</t>
+  </si>
+  <si>
+    <t>Fokas, A. S.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.05.08.20095489v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Better Strategies for Containing COVID-19 Epidemics --- A Study of 25 Countries via an Extended Varying Coefficient SEIR Model 
+</t>
+  </si>
+  <si>
+    <t>Gu, J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.27.20081232v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+COVID-19 Disease Dynamics in Germany: First Models and Parameter Identification 
+</t>
+  </si>
+  <si>
+    <t>Goetz, T.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.23.20076992v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SIR-simulation of Corona pandemic dynamics in Europe 
+</t>
+  </si>
+  <si>
+    <t>Nesteruk, I.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.22.20075135v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nonlinear Markov Chain Modelling of the Novel Coronavirus (Covid-19) Pandemic 
+</t>
+  </si>
+  <si>
+    <t>Catak, M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.21.20073668v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The impact of current and future control measures on the spread of COVID-19 in Germany 
+</t>
+  </si>
+  <si>
+    <t>Barbarossa, M. V.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.18.20069955v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A model-based evaluation of the efficacy of COVID-19 social distancing, testing and hospital triage policies 
+</t>
+  </si>
+  <si>
+    <t>McCombs, A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.20.20073213v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Modeling Exit Strategies from COVID-19 Lockdown with a Focus on Antibody Tests 
+</t>
+  </si>
+  <si>
+    <t>German, R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.14.20063750v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The end of the social confinement in Spain and the COVID-19 re-emergence risk 
+</t>
+  </si>
+  <si>
+    <t>Lopez, L.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.14.20064766v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The December 2019 New Corona Virus Disease (SARS-CoV-2) Outbreak: A Behavioral Infectious Disease Policy Model 
+</t>
+  </si>
+  <si>
+    <t>Struben, J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.13.20063610v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Estimating the Final Epidemic Size for COVID-19 Outbreak using Improved Epidemiological Models 
+</t>
+  </si>
+  <si>
+    <t>Ranjan, R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.12.20061002v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Intervention strategies against COVID-19 and their estimated impact on Swedish healthcare capacity 
+</t>
+  </si>
+  <si>
+    <t>Gardner, J. M.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.11.20062133v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Should contact bans be lifted in Germany? A quantitative prediction of its effects 
+</t>
+  </si>
+  <si>
+    <t>Donsimoni, J. R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.10.20060301v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+An agent-based epidemic model REINA for COVID-19 to identify destructive policies 
+</t>
+  </si>
+  <si>
+    <t>Tuomisto, J. T.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.09.20047498v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A first study on the impact of current and future control measures on the spread of COVID-19 in Germany 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.04.08.20056630v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A modified SEIR model to predict the COVID-19 outbreak in Spain: simulating control scenarios and multi-scale epidemics 
+</t>
+  </si>
+  <si>
+    <t>Lopez, L. R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.03.27.20045005v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Forecasting the Worldwide Spread of COVID-19 based on Logistic Model and SEIR Model 
+</t>
+  </si>
+  <si>
+    <t>Zhou, X.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.03.26.20044289v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Projecting the Spread of COVID19 for Germany 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.03.26.20044214v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Predicting the number of reported and unreported cases for the COVID-19 epidemic in South Korea, Italy, France and Germany 
+</t>
+  </si>
+  <si>
+    <t>magal, p.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.03.21.20040154v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Covid-19 health care demand and mortality in Sweden in response to non-pharmaceutical (NPIs) mitigation and suppression scenarios 
+</t>
+  </si>
+  <si>
+    <t>Rocklov, J.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.03.20.20039594v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Lessons drawn from China and South Korea for managing COVID-19 epidemic: insights from a comparative modeling study 
+</t>
+  </si>
+  <si>
+    <t>Tang, B.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.03.09.20033464v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Evaluation of the incidence of COVID-19 and of the efficacy of contention measures in Spain: a data-driven approach. 
+</t>
+  </si>
+  <si>
+    <t>Aleta, A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.medrxiv.org/content/10.1101/2020.03.01.20029801v1?rss=1"
+</t>
+  </si>
+  <si>
+    <t>medrxiv</t>
+  </si>
+  <si>
+    <t>arxiv</t>
+  </si>
+  <si>
+    <t>COVID-19 infection and recovery in various countries: Modeling the
+  dynamics and evaluating the non-pharmaceutical mitigation scenarios</t>
+  </si>
+  <si>
+    <t>Yong Zhang</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2003.13901v1</t>
+  </si>
+  <si>
+    <t>Global analysis of the COVID-19 pandemic using simple epidemiological
+  models</t>
+  </si>
+  <si>
+    <t>J. E. Amaro</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2005.06742v1</t>
+  </si>
+  <si>
+    <t>Robust and optimal predictive control of the COVID-19 outbreak</t>
+  </si>
+  <si>
+    <t>J. Köhler</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2005.03580v1</t>
+  </si>
+  <si>
+    <t>Model studies on the COVID-19 pandemic in Sweden</t>
+  </si>
+  <si>
+    <t>Chong Qi</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2004.01575v1</t>
+  </si>
+  <si>
+    <t>The D model for deaths by COVID-19</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2003.13747v1</t>
+  </si>
+  <si>
+    <t>Accounting for Symptomatic and Asymptomatic in a SEIR-type model of
+  COVID-19</t>
+  </si>
+  <si>
+    <t>Jayrold P. Arcede</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2004.01805v2</t>
+  </si>
+  <si>
+    <t>An Epidemic Model SIPHERD and its application for prediction of the
+  spread of COVID-19 infection for India and USA</t>
+  </si>
+  <si>
+    <t>Ashutosh Mahajan</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2005.00921v2</t>
+  </si>
+  <si>
+    <t>Robust predictive model for Carriers, Infections and Recoveries (CIR):
+  predicting death rates for CoVid-19 in Spain</t>
+  </si>
+  <si>
+    <t>Efren M. Benavides</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2003.13890v2</t>
+  </si>
+  <si>
+    <t>A Semiempirical Dynamical Model to Forecast the Propagation of
+  Epidemics: The Case of the Sars-Cov-2 in Spain</t>
+  </si>
+  <si>
+    <t>Juan C. Mora</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2004.08990v1</t>
+  </si>
+  <si>
+    <t>Did lockdowns serve their purpose?</t>
+  </si>
+  <si>
+    <t>Serena Bradde</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2006.09829v1</t>
+  </si>
+  <si>
+    <t>COVID-19: Development of a Robust Mathematical Model and Simulation
+  Package with Consideration for Ageing Population and Time Delay for Control
+  Action and Resusceptibility</t>
+  </si>
+  <si>
+    <t>Kok Yew Ng</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2004.01974v4</t>
+  </si>
+  <si>
+    <t>Beyond just "flattening the curve": Optimal control of epidemics with
+  purely non-pharmaceutical interventions</t>
+  </si>
+  <si>
+    <t>Markus Kantner</t>
+  </si>
+  <si>
+    <t>http://arxiv.org/abs/2004.09471v2</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Transmission model?</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Baseline projection of deaths and/or cases explicitly reported?</t>
+  </si>
+  <si>
+    <t>No - percent reduction attributable to intervention</t>
+  </si>
+  <si>
+    <t>Uses Imperial model</t>
+  </si>
+  <si>
+    <t>Assumes random mixing across whole population, simple SEIR</t>
+  </si>
+  <si>
+    <t>No - projects second wave</t>
+  </si>
+  <si>
+    <t>No - shows changes in effective contact rate with interventions</t>
+  </si>
+  <si>
+    <t>stochastic SEIR model combined with poisson model somehow - not sure</t>
+  </si>
+  <si>
+    <t>basic SIR with random mixing</t>
+  </si>
+  <si>
+    <t>No - only fit to observed cases/deaths/tests</t>
+  </si>
+  <si>
+    <t>basic SEIR model but accounts for severity of disease</t>
+  </si>
+  <si>
+    <t>No - fit to data assuming measures as of 15 May</t>
+  </si>
+  <si>
+    <t>SEIR model accounting for asymptomatic cases</t>
+  </si>
+  <si>
+    <t>No - seem to compare suppression to mitigation but not no intervention</t>
+  </si>
+  <si>
+    <t>SEIR model in two stages pre and post lockdown</t>
+  </si>
+  <si>
+    <t>No - only projects forward to lift lockdown</t>
+  </si>
+  <si>
+    <t>Model type</t>
+  </si>
+  <si>
+    <t>modified SIR model in two phases</t>
+  </si>
+  <si>
+    <t>SIR model with hospitalization fit to data from China</t>
+  </si>
+  <si>
+    <t>Not really clear, if anything, cases only and not deaths</t>
+  </si>
+  <si>
+    <t>Some combo of SIR with autoregressive time series</t>
+  </si>
+  <si>
+    <t>sort of</t>
   </si>
 </sst>
 </file>
@@ -717,7 +1370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -745,6 +1398,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,7 +1720,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:N1"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1976,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="153" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1389,7 +2046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="204" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -1681,11 +2338,1237 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D95D189-4E51-2E4F-AB4D-8AA53F517910}">
+  <dimension ref="A1:N47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="65.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="7.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E1" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" t="s">
+        <v>340</v>
+      </c>
+      <c r="H1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I1" t="s">
+        <v>342</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" t="s">
+        <v>345</v>
+      </c>
+      <c r="M1" t="s">
+        <v>360</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="M2" t="s">
+        <v>347</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="M3" t="s">
+        <v>348</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>297</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>297</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>297</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>297</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>297</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>297</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>297</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>297</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>297</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>297</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>297</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>297</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>297</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>297</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>297</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>297</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>298</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>298</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>298</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>298</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>298</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>298</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>298</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>298</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>298</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>298</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70F69A0-FAED-784F-B2D4-C2A53A6FD9D8}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G20" zoomScale="234" zoomScaleNormal="234" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated list structure to share with modelling course
</commit_message>
<xml_diff>
--- a/extraction.xlsx
+++ b/extraction.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jw12513/git/covid-litsearch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0024107-121B-C241-9BD4-59026F07E0B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EFBC95-D583-6949-A477-C5CA2410754B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{73474356-85FC-2C44-83A7-B203B79C5057}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="UK related" sheetId="1" r:id="rId1"/>
     <sheet name="Other countries" sheetId="3" r:id="rId2"/>
     <sheet name="UK" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -1720,7 +1720,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2342,8 +2342,8 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2998,7 +2998,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
     </row>
-    <row r="20" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>297</v>
       </c>
@@ -3038,7 +3038,7 @@
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>297</v>
       </c>
@@ -3058,7 +3058,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
-    <row r="23" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>297</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
     </row>
-    <row r="24" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>297</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>297</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
     </row>
-    <row r="26" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>297</v>
       </c>
@@ -3138,7 +3138,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>297</v>
       </c>
@@ -3158,7 +3158,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="28" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>297</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>297</v>
       </c>
@@ -3198,7 +3198,7 @@
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>297</v>
       </c>
@@ -3218,7 +3218,7 @@
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
     </row>
-    <row r="31" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>297</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>297</v>
       </c>
@@ -3258,7 +3258,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>297</v>
       </c>
@@ -3278,7 +3278,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>297</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
     </row>
-    <row r="35" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>297</v>
       </c>
@@ -3567,7 +3567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70F69A0-FAED-784F-B2D4-C2A53A6FD9D8}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>

</xml_diff>